<commit_message>
[PARAMETRAGE] : config MongoDB + dump
- mise en place du chargement des paramètres depuis la base mongo
- dump de la base de dev
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/suivi_garde_test.xlsx
+++ b/src/main/resources/testFiles/suivi_garde_test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\formation-workspaces\calcul-assmat-api\src\main\resources\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Projets\workspace\calcul-assmat-api\src\main\resources\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9D0086-3F25-4A02-A548-462E3E7E24BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
@@ -57,11 +58,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -70,6 +71,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -88,17 +96,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,75 +467,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="15" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>43346.79166195602</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>43346</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9">
         <v>0.38541666666424135</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="9">
         <v>0.70833333333575865</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>43347.328665138892</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>43347</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -465,12 +568,14 @@
       <c r="H3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>43347.794715173615</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>43347</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -485,12 +590,14 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>43349.921830497682</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>43349</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -501,15 +608,18 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>43349.922125462967</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>43349</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -521,12 +631,17 @@
       <c r="E6" s="4">
         <v>0.72916666666424135</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>43350.783449976851</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>43350</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -538,32 +653,41 @@
       <c r="E7" s="4">
         <v>0.76041666666424135</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>43350.783746875</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>43350</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="4">
         <v>0.76041666666424135</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>43353.883479074073</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>43353</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -572,18 +696,22 @@
       <c r="D9" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>43353.883786770835</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>43353</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -595,12 +723,17 @@
       <c r="E10" s="4">
         <v>0.71875</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>43354.774429189813</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>43354</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -609,15 +742,20 @@
       <c r="D11" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>43354.790583796297</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>43354</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -629,12 +767,17 @@
       <c r="E12" s="4">
         <v>0.77083333333575865</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>43356.868058912034</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>43356</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -643,15 +786,20 @@
       <c r="D13" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>43356.868448819441</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>43356</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -663,12 +811,17 @@
       <c r="E14" s="4">
         <v>0.72916666666424135</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>43357.862597106483</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>43357</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -680,12 +833,17 @@
       <c r="E15" s="4">
         <v>0.70833333333575865</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>43360.939879560188</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="5">
         <v>43360</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -694,15 +852,20 @@
       <c r="D16" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>43360.940077534724</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <v>43360</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -714,12 +877,17 @@
       <c r="E17" s="4">
         <v>0.70833333333575865</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>43361.832989317132</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>43361</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -728,15 +896,20 @@
       <c r="D18" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>43361.833331574075</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>43361</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -748,12 +921,17 @@
       <c r="E19" s="4">
         <v>0.73958333333575865</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>43363.782638321762</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>43363</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -762,15 +940,20 @@
       <c r="D20" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>43363.782996678245</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>43363</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -782,12 +965,17 @@
       <c r="E21" s="4">
         <v>0.71875</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>43364.972090138894</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>43364</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -799,12 +987,17 @@
       <c r="E22" s="4">
         <v>0.73958333333575865</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>43367.817552430555</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>43367</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -813,18 +1006,22 @@
       <c r="D23" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>43367.817830601853</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <v>43367</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -836,12 +1033,17 @@
       <c r="E24" s="4">
         <v>0.72916666666424135</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>43368.821946226853</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="5">
         <v>43368</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -850,18 +1052,22 @@
       <c r="D25" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>43368.822125300925</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="5">
         <v>43368</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -873,12 +1079,17 @@
       <c r="E26" s="4">
         <v>0.70833333333575865</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>43369.94543605324</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="5">
         <v>43370</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -887,18 +1098,22 @@
       <c r="D27" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>43369.945920196755</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="5">
         <v>43370</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -910,12 +1125,17 @@
       <c r="E28" s="4">
         <v>0.71875</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>43369.946309108796</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="5">
         <v>43371</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -927,8 +1147,14 @@
       <c r="E29" s="4">
         <v>0.70833333333575865</v>
       </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Calcul] : calcul par employé
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/suivi_garde_test.xlsx
+++ b/src/main/resources/testFiles/suivi_garde_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>Horodateur</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>employe1</t>
+  </si>
+  <si>
+    <t>maternelle2</t>
   </si>
 </sst>
 </file>
@@ -99,12 +102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,11 +426,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -620,6 +624,49 @@
         <v>0.72916666666424135</v>
       </c>
       <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43435.669681574072</v>
+      </c>
+      <c r="B10" s="5">
+        <v>43429</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43435.669681574072</v>
+      </c>
+      <c r="B11" s="5">
+        <v>43429</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.72916666666424135</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Dump base + fichier test]
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/suivi_garde_test.xlsx
+++ b/src/main/resources/testFiles/suivi_garde_test.xlsx
@@ -9,18 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
-    <sheet name="Réponses au formulaire 2" sheetId="1" r:id="rId1"/>
-    <sheet name="Réponses au formulaire 1" sheetId="2" r:id="rId2"/>
+    <sheet name="12-2018" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
   <si>
     <t>Horodateur</t>
   </si>
@@ -58,10 +57,10 @@
     <t>Joséphine</t>
   </si>
   <si>
-    <t>employe1</t>
-  </si>
-  <si>
-    <t>maternelle2</t>
+    <t>eda</t>
+  </si>
+  <si>
+    <t>uotap</t>
   </si>
 </sst>
 </file>
@@ -102,13 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,11 +424,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -472,53 +470,53 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43435.660487800924</v>
+        <v>43447.922826192131</v>
       </c>
       <c r="B2" s="2">
-        <v>43430</v>
+        <v>43437</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4">
         <v>0.32638888889050577</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43435.660703078705</v>
+        <v>43447.923079259257</v>
       </c>
       <c r="B3" s="2">
-        <v>43430</v>
+        <v>43437</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
         <v>0.32638888889050577</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43435.660997546292</v>
+        <v>43447.923749016205</v>
       </c>
       <c r="B4" s="2">
-        <v>43431</v>
+        <v>43438</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4">
         <v>0.31944444444525288</v>
@@ -526,73 +524,67 @@
       <c r="F4" s="4">
         <v>0.78125</v>
       </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43435.661190069441</v>
+        <v>43447.923980254629</v>
       </c>
       <c r="B5" s="2">
-        <v>43431</v>
+        <v>43438</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4">
         <v>0.31944444444525288</v>
       </c>
-      <c r="F5" s="4">
-        <v>0.78125</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43435.661438738425</v>
+        <v>43447.924275462967</v>
       </c>
       <c r="B6" s="2">
-        <v>43433</v>
+        <v>43440</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4">
         <v>0.32638888889050577</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43435.661619803243</v>
+        <v>43447.924916620366</v>
       </c>
       <c r="B7" s="2">
-        <v>43433</v>
+        <v>43440</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4">
         <v>0.32638888889050577</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43435.661820590278</v>
+        <v>43447.925302268515</v>
       </c>
       <c r="B8" s="2">
-        <v>43434</v>
+        <v>43441</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
@@ -604,35 +596,35 @@
         <v>0.375</v>
       </c>
       <c r="F8" s="4">
-        <v>0.72916666666424135</v>
+        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43435.669681574072</v>
+        <v>43447.925976620369</v>
       </c>
       <c r="B9" s="2">
-        <v>43434</v>
+        <v>43444</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.32638888889050577</v>
       </c>
       <c r="F9" s="4">
-        <v>0.72916666666424135</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
+        <v>0.69791666666424135</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43435.669681574072</v>
-      </c>
-      <c r="B10" s="5">
-        <v>43429</v>
+        <v>43447.926128391206</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43444</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -641,18 +633,15 @@
         <v>10</v>
       </c>
       <c r="E10" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
+        <v>0.32638888889050577</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43435.669681574072</v>
-      </c>
-      <c r="B11" s="5">
-        <v>43429</v>
+        <v>43447.926492638886</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43445</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -661,67 +650,221 @@
         <v>11</v>
       </c>
       <c r="E11" s="4">
+        <v>0.31944444444525288</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43447.926888206013</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43445</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.31944444444525288</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.78125</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43447.927182534724</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43447</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.69791666666424135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43447.927346840283</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43447</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43447.927615775465</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43448</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4">
         <v>0.375</v>
       </c>
-      <c r="F11" s="4">
-        <v>0.72916666666424135</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16" width="21.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
+      <c r="F15" s="4">
+        <v>0.69791666666424135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43453.899308101856</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43451</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43453.899680972223</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43451</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43453.900036192128</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43452</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.29861111110949423</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.69791666666424135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43453.90027283565</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43452</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.29861111110949423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43466.925266041668</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43454</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.69791666666424135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43466.925446388894</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43454</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.32638888889050577</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43466.925983553243</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43455</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.66666666666424135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>